<commit_message>
Se genera el archivo resultado_horarios.xlsx
</commit_message>
<xml_diff>
--- a/input/dias_franjas.xlsx
+++ b/input/dias_franjas.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/MacLeod/Playground/chorario/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{288D3CC6-1F27-C643-8ECF-0ACD8C6F33DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AF24D4F-1BF1-3846-9DB0-E5257292B83A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{19148547-FEF4-1448-88F6-2FCA983E4A15}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>S</t>
   </si>
@@ -43,6 +43,24 @@
   </si>
   <si>
     <t>M</t>
+  </si>
+  <si>
+    <t>FILTROS DEL CHORARIO</t>
+  </si>
+  <si>
+    <t>Centro de Idiomas Rocherau</t>
+  </si>
+  <si>
+    <t>Sede Principal Bogotá</t>
+  </si>
+  <si>
+    <t>Ordenar por NRC (curso)</t>
+  </si>
+  <si>
+    <t>Cupo 35 o 45</t>
+  </si>
+  <si>
+    <t>Para saber el día se concatena todos las columnas  DIA</t>
   </si>
 </sst>
 </file>
@@ -404,302 +422,326 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F37E0AC-A414-CD45-95C7-E7F8DE72B2B2}">
-  <dimension ref="B2:M20"/>
+  <dimension ref="B2:N20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="O17" sqref="O17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="8" width="10.83203125" style="1"/>
-    <col min="9" max="10" width="5.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.83203125" style="1"/>
-    <col min="12" max="13" width="5.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="10.83203125" style="1"/>
+    <col min="1" max="1" width="10.83203125" style="1"/>
+    <col min="2" max="3" width="5.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="3.33203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="2.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="3.83203125" style="1" customWidth="1"/>
+    <col min="7" max="8" width="5.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.83203125" style="1"/>
+    <col min="10" max="11" width="5.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="10.83203125" style="1"/>
+    <col min="14" max="14" width="22.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B2" s="1">
         <v>700</v>
       </c>
       <c r="C2" s="1">
         <v>829</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="I2" s="1">
+      <c r="G2" s="1">
         <v>700</v>
       </c>
-      <c r="J2" s="1">
+      <c r="H2" s="1">
         <v>829</v>
       </c>
-    </row>
-    <row r="3" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="N2" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B3" s="1">
         <v>745</v>
       </c>
       <c r="C3" s="1">
         <v>914</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="L3" s="1">
+      <c r="J3" s="1">
         <v>745</v>
       </c>
-      <c r="M3" s="1">
+      <c r="K3" s="1">
         <v>914</v>
       </c>
-    </row>
-    <row r="4" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="N3" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B4" s="1">
         <v>830</v>
       </c>
       <c r="C4" s="1">
         <v>959</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="1">
+      <c r="G4" s="1">
         <v>830</v>
       </c>
-      <c r="J4" s="1">
+      <c r="H4" s="1">
         <v>959</v>
       </c>
-    </row>
-    <row r="5" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="N4" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B5" s="1">
         <v>915</v>
       </c>
       <c r="C5" s="1">
         <v>1044</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="E5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="L5" s="1">
+      <c r="J5" s="1">
         <v>915</v>
       </c>
-      <c r="M5" s="1">
+      <c r="K5" s="1">
         <v>1044</v>
       </c>
-    </row>
-    <row r="6" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="N5" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B6" s="1">
         <v>1000</v>
       </c>
       <c r="C6" s="1">
         <v>1129</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="E6" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="I6" s="1">
+      <c r="G6" s="1">
         <v>1000</v>
       </c>
-      <c r="J6" s="1">
+      <c r="H6" s="1">
         <v>1129</v>
       </c>
-    </row>
-    <row r="7" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="N6" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B7" s="1">
         <v>1045</v>
       </c>
       <c r="C7" s="1">
         <v>1214</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="E7" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="L7" s="1">
+      <c r="J7" s="1">
         <v>1045</v>
       </c>
-      <c r="M7" s="1">
+      <c r="K7" s="1">
         <v>1214</v>
       </c>
-    </row>
-    <row r="8" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="N7" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B8" s="1">
         <v>1130</v>
       </c>
       <c r="C8" s="1">
         <v>1259</v>
       </c>
-      <c r="I8" s="1">
+      <c r="G8" s="1">
         <v>1130</v>
       </c>
-      <c r="J8" s="1">
+      <c r="H8" s="1">
         <v>1259</v>
       </c>
     </row>
-    <row r="9" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B9" s="1">
         <v>1215</v>
       </c>
       <c r="C9" s="1">
         <v>1344</v>
       </c>
-      <c r="L9" s="1">
+      <c r="J9" s="1">
         <v>1215</v>
       </c>
-      <c r="M9" s="1">
+      <c r="K9" s="1">
         <v>1344</v>
       </c>
     </row>
-    <row r="10" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B10" s="1">
         <v>1345</v>
       </c>
       <c r="C10" s="1">
         <v>1514</v>
       </c>
-      <c r="I10" s="1">
+      <c r="G10" s="1">
         <v>1345</v>
       </c>
-      <c r="J10" s="1">
+      <c r="H10" s="1">
         <v>1514</v>
       </c>
     </row>
-    <row r="11" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B11" s="1">
         <v>1430</v>
       </c>
       <c r="C11" s="1">
         <v>1559</v>
       </c>
-      <c r="L11" s="1">
+      <c r="J11" s="1">
         <v>1430</v>
       </c>
-      <c r="M11" s="1">
+      <c r="K11" s="1">
         <v>1559</v>
       </c>
     </row>
-    <row r="12" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B12" s="1">
         <v>1515</v>
       </c>
       <c r="C12" s="1">
         <v>1644</v>
       </c>
-      <c r="I12" s="1">
+      <c r="G12" s="1">
         <v>1515</v>
       </c>
-      <c r="J12" s="1">
+      <c r="H12" s="1">
         <v>1644</v>
       </c>
     </row>
-    <row r="13" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B13" s="1">
         <v>1600</v>
       </c>
       <c r="C13" s="1">
         <v>1729</v>
       </c>
-      <c r="L13" s="1">
+      <c r="J13" s="1">
         <v>1600</v>
       </c>
-      <c r="M13" s="1">
+      <c r="K13" s="1">
         <v>1729</v>
       </c>
     </row>
-    <row r="14" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B14" s="1">
         <v>1600</v>
       </c>
       <c r="C14" s="1">
         <v>1859</v>
       </c>
-      <c r="I14" s="1">
+      <c r="G14" s="1">
         <v>1600</v>
       </c>
-      <c r="J14" s="1">
+      <c r="H14" s="1">
         <v>1859</v>
       </c>
     </row>
-    <row r="15" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B15" s="1">
         <v>1645</v>
       </c>
       <c r="C15" s="1">
         <v>1814</v>
       </c>
-      <c r="L15" s="1">
+      <c r="J15" s="1">
         <v>1645</v>
       </c>
-      <c r="M15" s="1">
+      <c r="K15" s="1">
         <v>1814</v>
       </c>
     </row>
-    <row r="16" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B16" s="1">
         <v>1815</v>
       </c>
       <c r="C16" s="1">
         <v>1944</v>
       </c>
-      <c r="I16" s="1">
+      <c r="G16" s="1">
         <v>1815</v>
       </c>
-      <c r="J16" s="1">
+      <c r="H16" s="1">
         <v>1944</v>
       </c>
     </row>
-    <row r="17" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B17" s="1">
         <v>1815</v>
       </c>
       <c r="C17" s="1">
         <v>2114</v>
       </c>
-      <c r="L17" s="1">
+      <c r="J17" s="1">
         <v>1815</v>
       </c>
-      <c r="M17" s="1">
+      <c r="K17" s="1">
         <v>2114</v>
       </c>
     </row>
-    <row r="18" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B18" s="1">
         <v>1900</v>
       </c>
       <c r="C18" s="1">
         <v>2159</v>
       </c>
-      <c r="I18" s="1">
+      <c r="G18" s="1">
         <v>1900</v>
       </c>
-      <c r="J18" s="1">
+      <c r="H18" s="1">
         <v>2159</v>
       </c>
     </row>
-    <row r="19" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B19" s="1">
         <v>1945</v>
       </c>
       <c r="C19" s="1">
         <v>2114</v>
       </c>
-      <c r="L19" s="1">
+      <c r="J19" s="1">
         <v>1945</v>
       </c>
-      <c r="M19" s="1">
+      <c r="K19" s="1">
         <v>2114</v>
       </c>
     </row>
-    <row r="20" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B20" s="1">
         <v>2030</v>
       </c>
       <c r="C20" s="1">
         <v>2159</v>
       </c>
-      <c r="I20" s="1">
+      <c r="G20" s="1">
         <v>2030</v>
       </c>
-      <c r="J20" s="1">
+      <c r="H20" s="1">
         <v>2159</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Se genera el Excel de horario con la disponibilidad de cada profesor
</commit_message>
<xml_diff>
--- a/input/dias_franjas.xlsx
+++ b/input/dias_franjas.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/MacLeod/Playground/chorario/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19C9F361-B1C6-6C45-8826-253A7C29F1B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64D04CF5-73AD-154F-B07A-BB3AF7B7C59C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{19148547-FEF4-1448-88F6-2FCA983E4A15}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" activeTab="1" xr2:uid="{19148547-FEF4-1448-88F6-2FCA983E4A15}"/>
   </bookViews>
   <sheets>
-    <sheet name="franjas" sheetId="2" r:id="rId1"/>
-    <sheet name="disp1" sheetId="7" r:id="rId2"/>
-    <sheet name="disp2" sheetId="8" r:id="rId3"/>
+    <sheet name="franjas v1" sheetId="2" r:id="rId1"/>
+    <sheet name="franjas v2" sheetId="9" r:id="rId2"/>
+    <sheet name="disp1" sheetId="7" r:id="rId3"/>
+    <sheet name="disp2" sheetId="8" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2113" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2119" uniqueCount="39">
   <si>
     <t>S</t>
   </si>
@@ -523,7 +524,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F37E0AC-A414-CD45-95C7-E7F8DE72B2B2}">
   <dimension ref="B2:N20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K27" sqref="K27"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -848,6 +851,903 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF3B83FF-7F03-4A49-9643-35ADAA958F62}">
+  <dimension ref="A1:BI69"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="2.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="4.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="5.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="12" width="4.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="61" width="5.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="62" max="16384" width="10.83203125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:61" x14ac:dyDescent="0.2">
+      <c r="B1" s="1">
+        <v>700</v>
+      </c>
+      <c r="C1" s="1">
+        <v>715</v>
+      </c>
+      <c r="D1" s="1">
+        <v>730</v>
+      </c>
+      <c r="E1" s="1">
+        <v>745</v>
+      </c>
+      <c r="F1" s="1">
+        <v>800</v>
+      </c>
+      <c r="G1" s="1">
+        <v>815</v>
+      </c>
+      <c r="H1" s="1">
+        <v>830</v>
+      </c>
+      <c r="I1" s="1">
+        <v>845</v>
+      </c>
+      <c r="J1" s="1">
+        <v>900</v>
+      </c>
+      <c r="K1" s="1">
+        <v>915</v>
+      </c>
+      <c r="L1" s="1">
+        <v>930</v>
+      </c>
+      <c r="M1" s="1">
+        <v>945</v>
+      </c>
+      <c r="N1" s="1">
+        <v>1000</v>
+      </c>
+      <c r="O1" s="1">
+        <v>1015</v>
+      </c>
+      <c r="P1" s="1">
+        <v>1030</v>
+      </c>
+      <c r="Q1" s="1">
+        <v>1045</v>
+      </c>
+      <c r="R1" s="1">
+        <v>1100</v>
+      </c>
+      <c r="S1" s="1">
+        <v>1115</v>
+      </c>
+      <c r="T1" s="1">
+        <v>1130</v>
+      </c>
+      <c r="U1" s="1">
+        <v>1145</v>
+      </c>
+      <c r="V1" s="1">
+        <v>1200</v>
+      </c>
+      <c r="W1" s="1">
+        <v>1215</v>
+      </c>
+      <c r="X1" s="1">
+        <v>1230</v>
+      </c>
+      <c r="Y1" s="1">
+        <v>1245</v>
+      </c>
+      <c r="Z1" s="1">
+        <v>1300</v>
+      </c>
+      <c r="AA1" s="1">
+        <v>1315</v>
+      </c>
+      <c r="AB1" s="1">
+        <v>1330</v>
+      </c>
+      <c r="AC1" s="1">
+        <v>1345</v>
+      </c>
+      <c r="AD1" s="1">
+        <v>1400</v>
+      </c>
+      <c r="AE1" s="1">
+        <v>1415</v>
+      </c>
+      <c r="AF1" s="1">
+        <v>1430</v>
+      </c>
+      <c r="AG1" s="1">
+        <v>1445</v>
+      </c>
+      <c r="AH1" s="1">
+        <v>1500</v>
+      </c>
+      <c r="AI1" s="1">
+        <v>1515</v>
+      </c>
+      <c r="AJ1" s="1">
+        <v>1530</v>
+      </c>
+      <c r="AK1" s="1">
+        <v>1545</v>
+      </c>
+      <c r="AL1" s="1">
+        <v>1600</v>
+      </c>
+      <c r="AM1" s="1">
+        <v>1615</v>
+      </c>
+      <c r="AN1" s="1">
+        <v>1630</v>
+      </c>
+      <c r="AO1" s="1">
+        <v>1645</v>
+      </c>
+      <c r="AP1" s="1">
+        <v>1700</v>
+      </c>
+      <c r="AQ1" s="1">
+        <v>1715</v>
+      </c>
+      <c r="AR1" s="1">
+        <v>1730</v>
+      </c>
+      <c r="AS1" s="1">
+        <v>1745</v>
+      </c>
+      <c r="AT1" s="1">
+        <v>1800</v>
+      </c>
+      <c r="AU1" s="1">
+        <v>1815</v>
+      </c>
+      <c r="AV1" s="1">
+        <v>1830</v>
+      </c>
+      <c r="AW1" s="1">
+        <v>1845</v>
+      </c>
+      <c r="AX1" s="1">
+        <v>1900</v>
+      </c>
+      <c r="AY1" s="1">
+        <v>1915</v>
+      </c>
+      <c r="AZ1" s="1">
+        <v>1930</v>
+      </c>
+      <c r="BA1" s="1">
+        <v>1945</v>
+      </c>
+      <c r="BB1" s="1">
+        <v>2000</v>
+      </c>
+      <c r="BC1" s="1">
+        <v>2015</v>
+      </c>
+      <c r="BD1" s="1">
+        <v>2030</v>
+      </c>
+      <c r="BE1" s="1">
+        <v>2045</v>
+      </c>
+      <c r="BF1" s="1">
+        <v>2100</v>
+      </c>
+      <c r="BG1" s="1">
+        <v>2215</v>
+      </c>
+      <c r="BH1" s="1">
+        <v>2230</v>
+      </c>
+      <c r="BI1" s="1">
+        <v>2245</v>
+      </c>
+    </row>
+    <row r="2" spans="1:61" x14ac:dyDescent="0.2">
+      <c r="B2" s="1">
+        <v>715</v>
+      </c>
+      <c r="C2" s="1">
+        <v>730</v>
+      </c>
+      <c r="D2" s="1">
+        <v>745</v>
+      </c>
+      <c r="E2" s="1">
+        <v>800</v>
+      </c>
+      <c r="F2" s="1">
+        <v>815</v>
+      </c>
+      <c r="G2" s="1">
+        <v>830</v>
+      </c>
+      <c r="H2" s="1">
+        <v>845</v>
+      </c>
+      <c r="I2" s="1">
+        <v>900</v>
+      </c>
+      <c r="J2" s="1">
+        <v>915</v>
+      </c>
+      <c r="K2" s="1">
+        <v>930</v>
+      </c>
+      <c r="L2" s="1">
+        <v>945</v>
+      </c>
+      <c r="M2" s="1">
+        <v>1000</v>
+      </c>
+      <c r="N2" s="1">
+        <v>1015</v>
+      </c>
+      <c r="O2" s="1">
+        <v>1030</v>
+      </c>
+      <c r="P2" s="1">
+        <v>1045</v>
+      </c>
+      <c r="Q2" s="1">
+        <v>1100</v>
+      </c>
+      <c r="R2" s="1">
+        <v>1115</v>
+      </c>
+      <c r="S2" s="1">
+        <v>1130</v>
+      </c>
+      <c r="T2" s="1">
+        <v>1145</v>
+      </c>
+      <c r="U2" s="1">
+        <v>1200</v>
+      </c>
+      <c r="V2" s="1">
+        <v>1215</v>
+      </c>
+      <c r="W2" s="1">
+        <v>1230</v>
+      </c>
+      <c r="X2" s="1">
+        <v>1245</v>
+      </c>
+      <c r="Y2" s="1">
+        <v>1300</v>
+      </c>
+      <c r="Z2" s="1">
+        <v>1315</v>
+      </c>
+      <c r="AA2" s="1">
+        <v>1330</v>
+      </c>
+      <c r="AB2" s="1">
+        <v>1345</v>
+      </c>
+      <c r="AC2" s="1">
+        <v>1400</v>
+      </c>
+      <c r="AD2" s="1">
+        <v>1415</v>
+      </c>
+      <c r="AE2" s="1">
+        <v>1430</v>
+      </c>
+      <c r="AF2" s="1">
+        <v>1445</v>
+      </c>
+      <c r="AG2" s="1">
+        <v>1500</v>
+      </c>
+      <c r="AH2" s="1">
+        <v>1515</v>
+      </c>
+      <c r="AI2" s="1">
+        <v>1530</v>
+      </c>
+      <c r="AJ2" s="1">
+        <v>1545</v>
+      </c>
+      <c r="AK2" s="1">
+        <v>1600</v>
+      </c>
+      <c r="AL2" s="1">
+        <v>1615</v>
+      </c>
+      <c r="AM2" s="1">
+        <v>1630</v>
+      </c>
+      <c r="AN2" s="1">
+        <v>1645</v>
+      </c>
+      <c r="AO2" s="1">
+        <v>1700</v>
+      </c>
+      <c r="AP2" s="1">
+        <v>1715</v>
+      </c>
+      <c r="AQ2" s="1">
+        <v>1730</v>
+      </c>
+      <c r="AR2" s="1">
+        <v>1745</v>
+      </c>
+      <c r="AS2" s="1">
+        <v>1800</v>
+      </c>
+      <c r="AT2" s="1">
+        <v>1815</v>
+      </c>
+      <c r="AU2" s="1">
+        <v>1830</v>
+      </c>
+      <c r="AV2" s="1">
+        <v>1845</v>
+      </c>
+      <c r="AW2" s="1">
+        <v>1900</v>
+      </c>
+      <c r="AX2" s="1">
+        <v>1915</v>
+      </c>
+      <c r="AY2" s="1">
+        <v>1930</v>
+      </c>
+      <c r="AZ2" s="1">
+        <v>1945</v>
+      </c>
+      <c r="BA2" s="1">
+        <v>2000</v>
+      </c>
+      <c r="BB2" s="1">
+        <v>2015</v>
+      </c>
+      <c r="BC2" s="1">
+        <v>2030</v>
+      </c>
+      <c r="BD2" s="1">
+        <v>2045</v>
+      </c>
+      <c r="BE2" s="1">
+        <v>2100</v>
+      </c>
+      <c r="BF2" s="1">
+        <v>2215</v>
+      </c>
+      <c r="BG2" s="1">
+        <v>2230</v>
+      </c>
+      <c r="BH2" s="1">
+        <v>2245</v>
+      </c>
+      <c r="BI2" s="1">
+        <v>2300</v>
+      </c>
+    </row>
+    <row r="3" spans="1:61" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:61" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:61" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:61" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:61" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:61" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:61" x14ac:dyDescent="0.2">
+      <c r="D10" s="1">
+        <v>700</v>
+      </c>
+      <c r="E10" s="1">
+        <v>715</v>
+      </c>
+    </row>
+    <row r="11" spans="1:61" x14ac:dyDescent="0.2">
+      <c r="D11" s="1">
+        <v>715</v>
+      </c>
+      <c r="E11" s="1">
+        <v>730</v>
+      </c>
+    </row>
+    <row r="12" spans="1:61" x14ac:dyDescent="0.2">
+      <c r="D12" s="1">
+        <v>730</v>
+      </c>
+      <c r="E12" s="1">
+        <v>745</v>
+      </c>
+    </row>
+    <row r="13" spans="1:61" x14ac:dyDescent="0.2">
+      <c r="D13" s="1">
+        <v>745</v>
+      </c>
+      <c r="E13" s="1">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="14" spans="1:61" x14ac:dyDescent="0.2">
+      <c r="D14" s="1">
+        <v>800</v>
+      </c>
+      <c r="E14" s="1">
+        <v>815</v>
+      </c>
+    </row>
+    <row r="15" spans="1:61" x14ac:dyDescent="0.2">
+      <c r="D15" s="1">
+        <v>815</v>
+      </c>
+      <c r="E15" s="1">
+        <v>830</v>
+      </c>
+    </row>
+    <row r="16" spans="1:61" x14ac:dyDescent="0.2">
+      <c r="D16" s="1">
+        <v>830</v>
+      </c>
+      <c r="E16" s="1">
+        <v>845</v>
+      </c>
+    </row>
+    <row r="17" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D17" s="1">
+        <v>845</v>
+      </c>
+      <c r="E17" s="1">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="18" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D18" s="1">
+        <v>900</v>
+      </c>
+      <c r="E18" s="1">
+        <v>915</v>
+      </c>
+    </row>
+    <row r="19" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D19" s="1">
+        <v>915</v>
+      </c>
+      <c r="E19" s="1">
+        <v>930</v>
+      </c>
+    </row>
+    <row r="20" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D20" s="1">
+        <v>930</v>
+      </c>
+      <c r="E20" s="1">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="21" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D21" s="1">
+        <v>945</v>
+      </c>
+      <c r="E21" s="1">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="22" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D22" s="1">
+        <v>1000</v>
+      </c>
+      <c r="E22" s="1">
+        <v>1015</v>
+      </c>
+    </row>
+    <row r="23" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D23" s="1">
+        <v>1015</v>
+      </c>
+      <c r="E23" s="1">
+        <v>1030</v>
+      </c>
+    </row>
+    <row r="24" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D24" s="1">
+        <v>1030</v>
+      </c>
+      <c r="E24" s="1">
+        <v>1045</v>
+      </c>
+    </row>
+    <row r="25" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D25" s="1">
+        <v>1045</v>
+      </c>
+      <c r="E25" s="1">
+        <v>1100</v>
+      </c>
+    </row>
+    <row r="26" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D26" s="1">
+        <v>1100</v>
+      </c>
+      <c r="E26" s="1">
+        <v>1115</v>
+      </c>
+    </row>
+    <row r="27" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D27" s="1">
+        <v>1115</v>
+      </c>
+      <c r="E27" s="1">
+        <v>1130</v>
+      </c>
+    </row>
+    <row r="28" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D28" s="1">
+        <v>1130</v>
+      </c>
+      <c r="E28" s="1">
+        <v>1145</v>
+      </c>
+    </row>
+    <row r="29" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D29" s="1">
+        <v>1145</v>
+      </c>
+      <c r="E29" s="1">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="30" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D30" s="1">
+        <v>1200</v>
+      </c>
+      <c r="E30" s="1">
+        <v>1215</v>
+      </c>
+    </row>
+    <row r="31" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D31" s="1">
+        <v>1215</v>
+      </c>
+      <c r="E31" s="1">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="32" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D32" s="1">
+        <v>1230</v>
+      </c>
+      <c r="E32" s="1">
+        <v>1245</v>
+      </c>
+    </row>
+    <row r="33" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D33" s="1">
+        <v>1245</v>
+      </c>
+      <c r="E33" s="1">
+        <v>1300</v>
+      </c>
+    </row>
+    <row r="34" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D34" s="1">
+        <v>1300</v>
+      </c>
+      <c r="E34" s="1">
+        <v>1315</v>
+      </c>
+    </row>
+    <row r="35" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D35" s="1">
+        <v>1315</v>
+      </c>
+      <c r="E35" s="1">
+        <v>1330</v>
+      </c>
+    </row>
+    <row r="36" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D36" s="1">
+        <v>1330</v>
+      </c>
+      <c r="E36" s="1">
+        <v>1345</v>
+      </c>
+    </row>
+    <row r="37" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D37" s="1">
+        <v>1345</v>
+      </c>
+      <c r="E37" s="1">
+        <v>1400</v>
+      </c>
+    </row>
+    <row r="38" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D38" s="1">
+        <v>1400</v>
+      </c>
+      <c r="E38" s="1">
+        <v>1415</v>
+      </c>
+    </row>
+    <row r="39" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D39" s="1">
+        <v>1415</v>
+      </c>
+      <c r="E39" s="1">
+        <v>1430</v>
+      </c>
+    </row>
+    <row r="40" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D40" s="1">
+        <v>1430</v>
+      </c>
+      <c r="E40" s="1">
+        <v>1445</v>
+      </c>
+    </row>
+    <row r="41" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D41" s="1">
+        <v>1445</v>
+      </c>
+      <c r="E41" s="1">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="42" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D42" s="1">
+        <v>1500</v>
+      </c>
+      <c r="E42" s="1">
+        <v>1515</v>
+      </c>
+    </row>
+    <row r="43" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D43" s="1">
+        <v>1515</v>
+      </c>
+      <c r="E43" s="1">
+        <v>1530</v>
+      </c>
+    </row>
+    <row r="44" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D44" s="1">
+        <v>1530</v>
+      </c>
+      <c r="E44" s="1">
+        <v>1545</v>
+      </c>
+    </row>
+    <row r="45" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D45" s="1">
+        <v>1545</v>
+      </c>
+      <c r="E45" s="1">
+        <v>1600</v>
+      </c>
+    </row>
+    <row r="46" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D46" s="1">
+        <v>1600</v>
+      </c>
+      <c r="E46" s="1">
+        <v>1615</v>
+      </c>
+    </row>
+    <row r="47" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D47" s="1">
+        <v>1615</v>
+      </c>
+      <c r="E47" s="1">
+        <v>1630</v>
+      </c>
+    </row>
+    <row r="48" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D48" s="1">
+        <v>1630</v>
+      </c>
+      <c r="E48" s="1">
+        <v>1645</v>
+      </c>
+    </row>
+    <row r="49" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D49" s="1">
+        <v>1645</v>
+      </c>
+      <c r="E49" s="1">
+        <v>1700</v>
+      </c>
+    </row>
+    <row r="50" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D50" s="1">
+        <v>1700</v>
+      </c>
+      <c r="E50" s="1">
+        <v>1715</v>
+      </c>
+    </row>
+    <row r="51" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D51" s="1">
+        <v>1715</v>
+      </c>
+      <c r="E51" s="1">
+        <v>1730</v>
+      </c>
+    </row>
+    <row r="52" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D52" s="1">
+        <v>1730</v>
+      </c>
+      <c r="E52" s="1">
+        <v>1745</v>
+      </c>
+    </row>
+    <row r="53" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D53" s="1">
+        <v>1745</v>
+      </c>
+      <c r="E53" s="1">
+        <v>1800</v>
+      </c>
+    </row>
+    <row r="54" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D54" s="1">
+        <v>1800</v>
+      </c>
+      <c r="E54" s="1">
+        <v>1815</v>
+      </c>
+    </row>
+    <row r="55" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D55" s="1">
+        <v>1815</v>
+      </c>
+      <c r="E55" s="1">
+        <v>1830</v>
+      </c>
+    </row>
+    <row r="56" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D56" s="1">
+        <v>1830</v>
+      </c>
+      <c r="E56" s="1">
+        <v>1845</v>
+      </c>
+    </row>
+    <row r="57" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D57" s="1">
+        <v>1845</v>
+      </c>
+      <c r="E57" s="1">
+        <v>1900</v>
+      </c>
+    </row>
+    <row r="58" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D58" s="1">
+        <v>1900</v>
+      </c>
+      <c r="E58" s="1">
+        <v>1915</v>
+      </c>
+    </row>
+    <row r="59" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D59" s="1">
+        <v>1915</v>
+      </c>
+      <c r="E59" s="1">
+        <v>1930</v>
+      </c>
+    </row>
+    <row r="60" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D60" s="1">
+        <v>1930</v>
+      </c>
+      <c r="E60" s="1">
+        <v>1945</v>
+      </c>
+    </row>
+    <row r="61" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D61" s="1">
+        <v>1945</v>
+      </c>
+      <c r="E61" s="1">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="62" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D62" s="1">
+        <v>2000</v>
+      </c>
+      <c r="E62" s="1">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="63" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D63" s="1">
+        <v>2015</v>
+      </c>
+      <c r="E63" s="1">
+        <v>2030</v>
+      </c>
+    </row>
+    <row r="64" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D64" s="1">
+        <v>2030</v>
+      </c>
+      <c r="E64" s="1">
+        <v>2045</v>
+      </c>
+    </row>
+    <row r="65" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D65" s="1">
+        <v>2045</v>
+      </c>
+      <c r="E65" s="1">
+        <v>2100</v>
+      </c>
+    </row>
+    <row r="66" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D66" s="1">
+        <v>2100</v>
+      </c>
+      <c r="E66" s="1">
+        <v>2115</v>
+      </c>
+    </row>
+    <row r="67" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D67" s="1">
+        <v>2115</v>
+      </c>
+      <c r="E67" s="1">
+        <v>2130</v>
+      </c>
+    </row>
+    <row r="68" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D68" s="1">
+        <v>2130</v>
+      </c>
+      <c r="E68" s="1">
+        <v>2145</v>
+      </c>
+    </row>
+    <row r="69" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D69" s="1">
+        <v>2145</v>
+      </c>
+      <c r="E69" s="1">
+        <v>2200</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA95F014-026B-DC44-BA35-4B9AAA6E127A}">
   <dimension ref="A1:E351"/>
   <sheetViews>
@@ -6829,7 +7729,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FE2007D-278F-9A4D-A5B2-73489C4A64AC}">
   <dimension ref="A1:E348"/>
   <sheetViews>

</xml_diff>

<commit_message>
- Se muestra el resultado del proceso en la Terminal usando tablas. - Se genera un archivo de Excel con el horario de todos los cursos sin asignar.
</commit_message>
<xml_diff>
--- a/input/dias_franjas.xlsx
+++ b/input/dias_franjas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/MacLeod/Playground/chorario/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FE6B670-D26A-9240-AAE9-46C3FB8ABC93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F977D7FC-FA4D-6B42-953E-FAFF8A8ACB8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="12800" windowHeight="15540" activeTab="1" xr2:uid="{19148547-FEF4-1448-88F6-2FCA983E4A15}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" activeTab="1" xr2:uid="{19148547-FEF4-1448-88F6-2FCA983E4A15}"/>
   </bookViews>
   <sheets>
     <sheet name="franjas v1" sheetId="2" r:id="rId1"/>
@@ -756,7 +756,7 @@
   <dimension ref="A1:BI69"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -764,9 +764,7 @@
     <col min="1" max="1" width="2.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="4.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="5.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="4.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="12" width="4.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="12" width="4.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="61" width="5.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="62" max="16384" width="10.83203125" style="1"/>
   </cols>

</xml_diff>